<commit_message>
reduce cool load to zero
</commit_message>
<xml_diff>
--- a/src/data/W_data.xlsx
+++ b/src/data/W_data.xlsx
@@ -4,14 +4,27 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView windowWidth="22188" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -39,7 +52,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -1003,11 +1016,11 @@
   <sheetPr/>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -1183,7 +1196,7 @@
         <v>199.54</v>
       </c>
       <c r="E9">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F9">
         <v>107.38</v>
@@ -1203,7 +1216,7 @@
         <v>239.44</v>
       </c>
       <c r="E10">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="F10">
         <v>39.51</v>
@@ -1223,7 +1236,7 @@
         <v>266.05</v>
       </c>
       <c r="E11">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="F11">
         <v>83.28</v>
@@ -1243,7 +1256,7 @@
         <v>279.35</v>
       </c>
       <c r="E12">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="F12">
         <v>128.02</v>
@@ -1263,7 +1276,7 @@
         <v>266.05</v>
       </c>
       <c r="E13">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <v>156.9</v>
@@ -1283,7 +1296,7 @@
         <v>248.75</v>
       </c>
       <c r="E14">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="F14">
         <v>145.77</v>
@@ -1303,7 +1316,7 @@
         <v>234.12</v>
       </c>
       <c r="E15">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <v>169.98</v>
@@ -1323,7 +1336,7 @@
         <v>219.49</v>
       </c>
       <c r="E16">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>165.62</v>
@@ -1343,7 +1356,7 @@
         <v>219.49</v>
       </c>
       <c r="E17">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>130.25</v>
@@ -1363,7 +1376,7 @@
         <v>218.16</v>
       </c>
       <c r="E18">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1383,7 +1396,7 @@
         <v>214.17</v>
       </c>
       <c r="E19">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1403,7 +1416,7 @@
         <v>212.84</v>
       </c>
       <c r="E20">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1525,7 +1538,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1542,7 +1555,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
modified the model and milp
</commit_message>
<xml_diff>
--- a/src/data/W_data.xlsx
+++ b/src/data/W_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375"/>
+    <workbookView windowWidth="18350" windowHeight="7000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,16 +37,16 @@
     <t>E_PRICE</t>
   </si>
   <si>
-    <t>P_EL</t>
+    <t>L_Power</t>
   </si>
   <si>
-    <t>H_TL</t>
+    <t>L_Heat</t>
   </si>
   <si>
-    <t>C_TL</t>
+    <t>L_Cool</t>
   </si>
   <si>
-    <t>P_RES</t>
+    <t>P_PV</t>
   </si>
 </sst>
 </file>
@@ -1017,10 +1017,10 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -1538,7 +1538,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1555,7 +1555,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>